<commit_message>
Bugfix in organoid death dynamics
</commit_message>
<xml_diff>
--- a/demos/organoid_demo/example_output/organoid_dynamics/results/AUC_delta.xlsx
+++ b/demos/organoid_demo/example_output/organoid_dynamics/results/AUC_delta.xlsx
@@ -47,7 +47,7 @@
     <t>well1</t>
   </si>
   <si>
-    <t>31/05/2019</t>
+    <t>02/05/2019</t>
   </si>
 </sst>
 </file>
@@ -142,10 +142,10 @@
         <v>11</v>
       </c>
       <c r="G2" t="n">
-        <v>-431.31003136868145</v>
+        <v>3009.474555884101</v>
       </c>
       <c r="H2" t="n">
-        <v>-18.95868269752446</v>
+        <v>64.10364515115018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>